<commit_message>
refactored 11, commentary, readers and wrappers
</commit_message>
<xml_diff>
--- a/input_files/output/AsimData.xlsx
+++ b/input_files/output/AsimData.xlsx
@@ -199,37 +199,37 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>4.412640795867052</v>
+        <v>5.126259292976878</v>
       </c>
       <c r="D3" t="n">
-        <v>4.412640795867052</v>
+        <v>5.126259292976878</v>
       </c>
       <c r="E3" t="n">
-        <v>5.67519896349711</v>
+        <v>6.388817460606935</v>
       </c>
       <c r="F3" t="n">
-        <v>4.305015410602002</v>
+        <v>5.001228578514028</v>
       </c>
       <c r="G3" t="n">
-        <v>5.385972253484967</v>
+        <v>6.063222416823513</v>
       </c>
       <c r="H3" t="n">
-        <v>4.110481136159656</v>
+        <v>4.775233946660782</v>
       </c>
       <c r="I3" t="n">
-        <v>5.199237279241688</v>
+        <v>5.853006762425328</v>
       </c>
       <c r="J3" t="n">
-        <v>3.9718667979049016</v>
+        <v>4.614202701995725</v>
       </c>
       <c r="K3" t="n">
-        <v>5.043749380344335</v>
+        <v>5.677967295125954</v>
       </c>
       <c r="L3" t="n">
-        <v>3.8606708300954926</v>
+        <v>4.485023965340245</v>
       </c>
       <c r="M3" t="n">
-        <v>4.965297677046992</v>
+        <v>5.589650812291744</v>
       </c>
     </row>
     <row r="4">
@@ -389,37 +389,37 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>64.14359718876827</v>
+        <v>66.02392186623553</v>
       </c>
       <c r="D8" t="n">
-        <v>56.422608638268386</v>
+        <v>58.302933315735636</v>
       </c>
       <c r="E8" t="n">
-        <v>76.76444385785462</v>
+        <v>78.64476853532187</v>
       </c>
       <c r="F8" t="n">
-        <v>104.87796830322546</v>
+        <v>106.71243140319352</v>
       </c>
       <c r="G8" t="n">
-        <v>9.86394460791993</v>
+        <v>11.648441786877179</v>
       </c>
       <c r="H8" t="n">
-        <v>33.47179588194267</v>
+        <v>35.223363588025556</v>
       </c>
       <c r="I8" t="n">
-        <v>27.20558735714596</v>
+        <v>28.928214920170046</v>
       </c>
       <c r="J8" t="n">
-        <v>53.45959394212214</v>
+        <v>55.15209498655532</v>
       </c>
       <c r="K8" t="n">
-        <v>65.97994907943591</v>
+        <v>67.65105990529806</v>
       </c>
       <c r="L8" t="n">
-        <v>77.9444171050631</v>
+        <v>79.58953506712467</v>
       </c>
       <c r="M8" t="n">
-        <v>51.962944736708735</v>
+        <v>53.6080626987703</v>
       </c>
     </row>
     <row r="9">
@@ -465,37 +465,37 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>18.839967269585575</v>
+        <v>84.31863285861598</v>
       </c>
       <c r="D10" t="n">
-        <v>20.970539505587915</v>
+        <v>86.44920509461834</v>
       </c>
       <c r="E10" t="n">
-        <v>26.869462266937937</v>
+        <v>92.34812785596833</v>
       </c>
       <c r="F10" t="n">
-        <v>16.53645159031786</v>
+        <v>80.4180765552256</v>
       </c>
       <c r="G10" t="n">
-        <v>13.561441397119602</v>
+        <v>75.70309992329442</v>
       </c>
       <c r="H10" t="n">
-        <v>13.3083906549509</v>
+        <v>74.30334405716413</v>
       </c>
       <c r="I10" t="n">
-        <v>12.50903938190705</v>
+        <v>72.49620834553139</v>
       </c>
       <c r="J10" t="n">
-        <v>12.716781943700592</v>
+        <v>71.6548532382814</v>
       </c>
       <c r="K10" t="n">
-        <v>18.977532955573434</v>
+        <v>77.17073131120219</v>
       </c>
       <c r="L10" t="n">
-        <v>13.514284083816799</v>
+        <v>70.80233129353206</v>
       </c>
       <c r="M10" t="n">
-        <v>14.653137505332948</v>
+        <v>71.9411847150482</v>
       </c>
     </row>
     <row r="11">
@@ -503,37 +503,37 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>20.842871939074396</v>
+        <v>93.28266885373951</v>
       </c>
       <c r="D11" t="n">
-        <v>23.199948447568833</v>
+        <v>95.63974536223392</v>
       </c>
       <c r="E11" t="n">
-        <v>29.725994376098413</v>
+        <v>102.16579129076352</v>
       </c>
       <c r="F11" t="n">
-        <v>18.29446611513567</v>
+        <v>88.96743871480895</v>
       </c>
       <c r="G11" t="n">
-        <v>23.58578418222825</v>
+        <v>92.33381200292212</v>
       </c>
       <c r="H11" t="n">
-        <v>23.069002540272812</v>
+        <v>90.54841736231234</v>
       </c>
       <c r="I11" t="n">
-        <v>21.734603793323263</v>
+        <v>88.09909516039598</v>
       </c>
       <c r="J11" t="n">
-        <v>22.03755643348846</v>
+        <v>87.24141904605743</v>
       </c>
       <c r="K11" t="n">
-        <v>33.23030866268789</v>
+        <v>97.61010982043769</v>
       </c>
       <c r="L11" t="n">
-        <v>23.468110664659317</v>
+        <v>86.8465327534069</v>
       </c>
       <c r="M11" t="n">
-        <v>25.561519367204884</v>
+        <v>88.93994145595246</v>
       </c>
     </row>
     <row r="12">
@@ -541,37 +541,37 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>85.79778721911651</v>
+        <v>383.98971969746793</v>
       </c>
       <c r="D12" t="n">
-        <v>95.5004783514195</v>
+        <v>393.6924108297709</v>
       </c>
       <c r="E12" t="n">
-        <v>122.36435304176257</v>
+        <v>420.556285520114</v>
       </c>
       <c r="F12" t="n">
-        <v>75.30750635622108</v>
+        <v>366.2264648716859</v>
       </c>
       <c r="G12" t="n">
-        <v>77.34577061412998</v>
+        <v>360.3408664462942</v>
       </c>
       <c r="H12" t="n">
-        <v>75.76327399058466</v>
+        <v>353.5362380975382</v>
       </c>
       <c r="I12" t="n">
-        <v>71.30565341697933</v>
+        <v>344.4891350327873</v>
       </c>
       <c r="J12" t="n">
-        <v>72.38451837576213</v>
+        <v>340.79037573065307</v>
       </c>
       <c r="K12" t="n">
-        <v>108.6442414205698</v>
+        <v>373.65792364301353</v>
       </c>
       <c r="L12" t="n">
-        <v>77.01205749257119</v>
+        <v>337.9036525136813</v>
       </c>
       <c r="M12" t="n">
-        <v>83.71208666194337</v>
+        <v>344.60368168305354</v>
       </c>
     </row>
     <row r="13">
@@ -731,37 +731,37 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>77.07289618184141</v>
+        <v>148.73258204571576</v>
       </c>
       <c r="D17" t="n">
-        <v>96.75083003447835</v>
+        <v>168.4105158983527</v>
       </c>
       <c r="E17" t="n">
-        <v>100.53169135487167</v>
+        <v>172.191377218746</v>
       </c>
       <c r="F17" t="n">
-        <v>112.38305857582903</v>
+        <v>182.29494722351131</v>
       </c>
       <c r="G17" t="n">
-        <v>108.47746114121189</v>
+        <v>176.485134923004</v>
       </c>
       <c r="H17" t="n">
-        <v>104.78008748812726</v>
+        <v>171.53281008509637</v>
       </c>
       <c r="I17" t="n">
-        <v>97.31542496068695</v>
+        <v>162.9652308192325</v>
       </c>
       <c r="J17" t="n">
-        <v>98.85007683667506</v>
+        <v>163.35175286197034</v>
       </c>
       <c r="K17" t="n">
-        <v>91.0420261522414</v>
+        <v>154.7285151187652</v>
       </c>
       <c r="L17" t="n">
-        <v>102.67926956447542</v>
+        <v>165.37516340826727</v>
       </c>
       <c r="M17" t="n">
-        <v>101.28969513391046</v>
+        <v>163.98558897770232</v>
       </c>
     </row>
     <row r="18">
@@ -769,37 +769,37 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>231.33760036950187</v>
+        <v>236.40176579265258</v>
       </c>
       <c r="D18" t="n">
-        <v>183.654338094223</v>
+        <v>188.7185035173737</v>
       </c>
       <c r="E18" t="n">
-        <v>218.5442727208129</v>
+        <v>223.6084381439636</v>
       </c>
       <c r="F18" t="n">
-        <v>156.49198517139723</v>
+        <v>161.432634364715</v>
       </c>
       <c r="G18" t="n">
-        <v>194.39108908664343</v>
+        <v>199.19716806847006</v>
       </c>
       <c r="H18" t="n">
-        <v>189.62349778699738</v>
+        <v>194.34088979899838</v>
       </c>
       <c r="I18" t="n">
-        <v>179.00978231311785</v>
+        <v>183.64923157747762</v>
       </c>
       <c r="J18" t="n">
-        <v>180.97521872230604</v>
+        <v>185.53353004511973</v>
       </c>
       <c r="K18" t="n">
-        <v>164.33219074535623</v>
+        <v>168.83289307830813</v>
       </c>
       <c r="L18" t="n">
-        <v>194.19734272375828</v>
+        <v>198.62804003912734</v>
       </c>
       <c r="M18" t="n">
-        <v>194.11142755629217</v>
+        <v>198.54212487166123</v>
       </c>
     </row>
     <row r="19">
@@ -807,37 +807,37 @@
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>3.5081599384155595</v>
+        <v>8.119159100686034</v>
       </c>
       <c r="D19" t="n">
-        <v>3.7999411325197547</v>
+        <v>8.410940294790228</v>
       </c>
       <c r="E19" t="n">
-        <v>3.5081599384155595</v>
+        <v>8.119159100686034</v>
       </c>
       <c r="F19" t="n">
-        <v>3.972063901588594</v>
+        <v>8.470599669657348</v>
       </c>
       <c r="G19" t="n">
-        <v>3.3293726282770812</v>
+        <v>7.705380184764197</v>
       </c>
       <c r="H19" t="n">
-        <v>3.792574981007444</v>
+        <v>8.08783171097124</v>
       </c>
       <c r="I19" t="n">
-        <v>3.2139412293155796</v>
+        <v>7.438229909453067</v>
       </c>
       <c r="J19" t="n">
-        <v>3.6646811277430933</v>
+        <v>7.815092485708791</v>
       </c>
       <c r="K19" t="n">
-        <v>3.117825406534985</v>
+        <v>7.215782908475841</v>
       </c>
       <c r="L19" t="n">
-        <v>3.562085097854271</v>
+        <v>7.596301973165214</v>
       </c>
       <c r="M19" t="n">
-        <v>3.069329992651097</v>
+        <v>7.10354686796204</v>
       </c>
     </row>
     <row r="21">

</xml_diff>